<commit_message>
Automatizacion del detalle de productos SVP, Inversiones, Creditos y CrediAgil
</commit_message>
<xml_diff>
--- a/SVP/src/test/resources/datadriven/consultasdedetalle/consulta_de_detalles.xlsx
+++ b/SVP/src/test/resources/datadriven/consultasdedetalle/consulta_de_detalles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Qv-3795\Documents\Proyecto Automatizacion SVP\svp-rediseno-personas-web-tests-bdd-screenplay\SVP\src\test\resources\datadriven\consultasdedetalle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F287AFC5-A93B-428A-9524-B927AEA708F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFB998D7-CA49-463D-A04A-3817B5D0730F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DetalleCuentasAhorro" sheetId="4" r:id="rId1"/>
@@ -20,7 +20,11 @@
     <sheet name="DetalleCreditos" sheetId="6" state="hidden" r:id="rId5"/>
     <sheet name="DetalleInversion" sheetId="7" state="hidden" r:id="rId6"/>
     <sheet name="DetalleCrediagil" sheetId="8" state="hidden" r:id="rId7"/>
-    <sheet name="Listas" sheetId="2" r:id="rId8"/>
+    <sheet name="DetalleFondosInversion" sheetId="10" r:id="rId8"/>
+    <sheet name="DetalleCreditos1" sheetId="11" r:id="rId9"/>
+    <sheet name="DetalleInversiones" sheetId="12" r:id="rId10"/>
+    <sheet name="DetalleCrediAgil1" sheetId="13" r:id="rId11"/>
+    <sheet name="Listas" sheetId="2" r:id="rId12"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -289,7 +293,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="116">
   <si>
     <t>Orientacion</t>
   </si>
@@ -565,6 +569,78 @@
   </si>
   <si>
     <t>****8091</t>
+  </si>
+  <si>
+    <t>Con fecha de vencimiento</t>
+  </si>
+  <si>
+    <t>Sin fecha de vencimiento</t>
+  </si>
+  <si>
+    <t>Tipo de fondo,Saldo disponible,Saldo total</t>
+  </si>
+  <si>
+    <t>Inversiones</t>
+  </si>
+  <si>
+    <t>Tipo de fondo,Saldo disponible,Saldo total,Fecha de vencimiento</t>
+  </si>
+  <si>
+    <t>0461000001260</t>
+  </si>
+  <si>
+    <t>FIDUQA04</t>
+  </si>
+  <si>
+    <t>Creditos</t>
+  </si>
+  <si>
+    <t>10001263181</t>
+  </si>
+  <si>
+    <t>Credito hipotecario</t>
+  </si>
+  <si>
+    <t>Tipo de credito,Capital vigente,Deuda a la fecha,Plan,Tasa de interes efectiva anual,Fecha de vencimiento,Numero de cuotas</t>
+  </si>
+  <si>
+    <t>29281026324</t>
+  </si>
+  <si>
+    <t>Credito de consumo</t>
+  </si>
+  <si>
+    <t>CHIPOTE95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tipo de credito,Capital vigente,Deuda a la fecha,Fecha de desembolso,Valor desembolsado, </t>
+  </si>
+  <si>
+    <t>27600103026</t>
+  </si>
+  <si>
+    <t>USUA13RIO</t>
+  </si>
+  <si>
+    <t>Inversion Virtual</t>
+  </si>
+  <si>
+    <t>CDT</t>
+  </si>
+  <si>
+    <t>Tipo de inversion,Fecha de apertura,Capital,Plazo en dias,Periodicidad de intereses al dia,Fecha de vencimiento,Tasa de interes efectiva anual,Tasa de interes nominal,Intereses pagados,Intereses del periodo</t>
+  </si>
+  <si>
+    <t>USUCAYCA01</t>
+  </si>
+  <si>
+    <t>CrediAgil</t>
+  </si>
+  <si>
+    <t>Crediagil</t>
+  </si>
+  <si>
+    <t>Cupo asignado,Cupo utilizado,Cupo disponible,Disponible con sobrecupo,Valor minimo a desembolsar,Valor maximo a desembolsar,Cupo de canje</t>
   </si>
 </sst>
 </file>
@@ -1152,6 +1228,282 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9957B2F-934D-49AA-8CBC-BF48D3D53632}">
+  <dimension ref="A1:N3"/>
+  <sheetViews>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="7" max="7" width="19.28515625" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="70.85546875" customWidth="1"/>
+    <col min="14" max="14" width="28.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="H2" s="11">
+        <v>1234</v>
+      </c>
+      <c r="I2" s="11">
+        <v>4321</v>
+      </c>
+      <c r="J2" s="4"/>
+      <c r="K2" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="L3" s="3"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3A5CDD7F-C493-48A7-A7F3-2F7B173DBE04}">
+          <x14:formula1>
+            <xm:f>Listas!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B3</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D32F815-7C8C-4C0C-80AE-BE49A6A447DF}">
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="7" max="7" width="19.28515625" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="70.85546875" customWidth="1"/>
+    <col min="14" max="14" width="28.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="H2" s="11">
+        <v>1234</v>
+      </c>
+      <c r="I2" s="11">
+        <v>4321</v>
+      </c>
+      <c r="J2" s="4"/>
+      <c r="K2" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="L2" s="3"/>
+      <c r="M2" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{29F321BB-262A-43DE-A654-9E532B084063}">
+          <x14:formula1>
+            <xm:f>Listas!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5B4D911-88F2-4FE9-9E98-33B11F0F3FDC}">
   <dimension ref="A1:N2"/>
@@ -1270,8 +1622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2212,8 +2564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:Q8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2417,29 +2769,289 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:A3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43CA1A8A-DFA9-4127-96CE-D3B8EE133DF0}">
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="7" max="7" width="19.28515625" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="70.85546875" customWidth="1"/>
+    <col min="14" max="14" width="28.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
+    <row r="1" spans="1:14">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>14</v>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="H2" s="11">
+        <v>1234</v>
+      </c>
+      <c r="I2" s="11">
+        <v>4321</v>
+      </c>
+      <c r="J2" s="4"/>
+      <c r="K2" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="11">
+        <v>1234</v>
+      </c>
+      <c r="I3" s="11">
+        <v>4321</v>
+      </c>
+      <c r="J3" s="4"/>
+      <c r="K3" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="L3" s="3"/>
+      <c r="M3" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{09632744-5D50-410A-B3D1-38CEC7053906}">
+          <x14:formula1>
+            <xm:f>Listas!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B3</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A6F8954-F988-4A25-B39A-FB9E0C6105B8}">
+  <dimension ref="A1:N3"/>
+  <sheetViews>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="7" max="7" width="19.28515625" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="70.85546875" customWidth="1"/>
+    <col min="14" max="14" width="28.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="H2" s="11">
+        <v>1234</v>
+      </c>
+      <c r="I2" s="11">
+        <v>4321</v>
+      </c>
+      <c r="J2" s="4"/>
+      <c r="K2" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="H3" s="11">
+        <v>1234</v>
+      </c>
+      <c r="I3" s="11">
+        <v>4321</v>
+      </c>
+      <c r="J3" s="4"/>
+      <c r="K3" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{79C9735E-F075-40CC-90AE-BD4CA86EA1F2}">
+          <x14:formula1>
+            <xm:f>Listas!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B3</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Automatización detalle de productos SVP - Ajustes por cambios en desarrollo y prueba final
</commit_message>
<xml_diff>
--- a/SVP/src/test/resources/datadriven/consultasdedetalle/consulta_de_detalles.xlsx
+++ b/SVP/src/test/resources/datadriven/consultasdedetalle/consulta_de_detalles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Qv-3795\Documents\Proyecto Automatizacion SVP\svp-rediseno-personas-web-tests-bdd-screenplay\SVP\src\test\resources\datadriven\consultasdedetalle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFB998D7-CA49-463D-A04A-3817B5D0730F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2870159-B830-47FB-9D91-D52682FFA5B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DetalleCuentasAhorro" sheetId="4" r:id="rId1"/>
@@ -293,7 +293,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="117">
   <si>
     <t>Orientacion</t>
   </si>
@@ -559,9 +559,6 @@
     <t>USUCTDC3</t>
   </si>
   <si>
-    <t>PRUEBAECARD02</t>
-  </si>
-  <si>
     <t>****7036</t>
   </si>
   <si>
@@ -640,7 +637,13 @@
     <t>Crediagil</t>
   </si>
   <si>
-    <t>Cupo asignado,Cupo utilizado,Cupo disponible,Disponible con sobrecupo,Valor minimo a desembolsar,Valor maximo a desembolsar,Cupo de canje</t>
+    <t>Cupo asignado,Cupo utilizado,Cupo disponible,Cupo de canje</t>
+  </si>
+  <si>
+    <t>FIDURENTA2</t>
+  </si>
+  <si>
+    <t>7001000083018</t>
   </si>
 </sst>
 </file>
@@ -1119,7 +1122,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1302,7 +1305,7 @@
       <c r="E2" s="9"/>
       <c r="F2" s="12"/>
       <c r="G2" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H2" s="11">
         <v>1234</v>
@@ -1312,16 +1315,16 @@
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -1340,12 +1343,12 @@
       <c r="I3" s="11"/>
       <c r="J3" s="4"/>
       <c r="K3" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L3" s="3"/>
       <c r="M3" s="7"/>
       <c r="N3" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1369,8 +1372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D32F815-7C8C-4C0C-80AE-BE49A6A447DF}">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1439,7 +1442,7 @@
       <c r="E2" s="9"/>
       <c r="F2" s="12"/>
       <c r="G2" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H2" s="11">
         <v>1234</v>
@@ -1449,14 +1452,16 @@
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="M2" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="L2" s="3"/>
-      <c r="M2" s="7" t="s">
-        <v>115</v>
-      </c>
       <c r="N2" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1622,8 +1627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1705,7 +1710,7 @@
         <v>75</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M2" s="7" t="s">
         <v>76</v>
@@ -1739,7 +1744,7 @@
         <v>75</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="M3" s="7" t="s">
         <v>76</v>
@@ -1773,7 +1778,7 @@
         <v>75</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="M4" s="7" t="s">
         <v>78</v>
@@ -1793,15 +1798,9 @@
       <c r="D5" s="7"/>
       <c r="E5" s="9"/>
       <c r="F5" s="12"/>
-      <c r="G5" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="H5" s="11">
-        <v>1234</v>
-      </c>
-      <c r="I5" s="11">
-        <v>1234</v>
-      </c>
+      <c r="G5" s="8"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
       <c r="J5" s="4"/>
       <c r="K5" s="3" t="s">
         <v>75</v>
@@ -2772,7 +2771,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43CA1A8A-DFA9-4127-96CE-D3B8EE133DF0}">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
@@ -2840,7 +2841,7 @@
       <c r="E2" s="9"/>
       <c r="F2" s="12"/>
       <c r="G2" s="8" t="s">
-        <v>98</v>
+        <v>115</v>
       </c>
       <c r="H2" s="11">
         <v>1234</v>
@@ -2850,16 +2851,16 @@
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="M2" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="L2" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="N2" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -2873,7 +2874,9 @@
       <c r="D3" s="7"/>
       <c r="E3" s="9"/>
       <c r="F3" s="12"/>
-      <c r="G3" s="8"/>
+      <c r="G3" s="8" t="s">
+        <v>97</v>
+      </c>
       <c r="H3" s="11">
         <v>1234</v>
       </c>
@@ -2882,14 +2885,16 @@
       </c>
       <c r="J3" s="4"/>
       <c r="K3" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="L3" s="3"/>
+        <v>94</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>96</v>
+      </c>
       <c r="M3" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -2983,7 +2988,7 @@
       <c r="E2" s="9"/>
       <c r="F2" s="12"/>
       <c r="G2" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H2" s="11">
         <v>1234</v>
@@ -2993,16 +2998,16 @@
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="N2" s="6" t="s">
         <v>100</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -3017,7 +3022,7 @@
       <c r="E3" s="9"/>
       <c r="F3" s="12"/>
       <c r="G3" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H3" s="11">
         <v>1234</v>
@@ -3027,16 +3032,16 @@
       </c>
       <c r="J3" s="4"/>
       <c r="K3" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L3" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="N3" s="6" t="s">
         <v>103</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>